<commit_message>
working on logic formatting
</commit_message>
<xml_diff>
--- a/notebooks/Questions_2024-05-31.xlsx
+++ b/notebooks/Questions_2024-05-31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABMI_Official\RCDST_Jupyter_webapp_Official\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BE4615-1C3E-4BF0-BC07-7924B9FBAF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBC7BCC-B8D2-4EC7-9B7F-2ADFE36FE604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="825" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3661" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3661" uniqueCount="899">
   <si>
     <t>Camera spacing</t>
   </si>
@@ -2792,6 +2792,15 @@
   </si>
   <si>
     <t>if objective=="obj_divers_rich"</t>
+  </si>
+  <si>
+    <t>{
+    "objective": [
+        "obj_divers_rich",
+        "obj_rel_abund",
+        "obj_behaviour"
+    ]
+}</t>
   </si>
 </sst>
 </file>
@@ -11070,8 +11079,8 @@
   <dimension ref="A1:AE63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -11736,7 +11745,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="78.75">
+    <row r="8" spans="1:31" ht="110.25">
       <c r="A8" s="64" t="s">
         <v>345</v>
       </c>
@@ -11763,7 +11772,7 @@
       </c>
       <c r="J8" s="146"/>
       <c r="K8" s="67" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="L8" s="65" t="s">
         <v>844</v>

</xml_diff>

<commit_message>
working on formatting question logics
</commit_message>
<xml_diff>
--- a/notebooks/Questions_2024-05-31.xlsx
+++ b/notebooks/Questions_2024-05-31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABMI_Official\RCDST_Jupyter_webapp_Official\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11222AF6-15FF-408A-90BD-9AC6F7F20FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBC5A9B-8C61-43CD-81D4-8886DAEC4081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="825" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11166,9 +11166,9 @@
   </sheetPr>
   <dimension ref="A1:AF63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -17030,7 +17030,7 @@
       <formula>"TRUE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:W2 P1:P63 AF1:AF63 U3:W48 Q3:T63 O45:AE45 I48:J48 W49:W63 I50:J53 U51:V63 K1:N63">
+  <conditionalFormatting sqref="Q1:W2 K1:N63 P1:P63 AF1:AF63 U3:W48 Q3:T63 O45:AE45 I48:J48 W49:W63 I50:J53 U51:V63">
     <cfRule type="cellIs" dxfId="66" priority="11" operator="equal">
       <formula>"-"</formula>
     </cfRule>

</xml_diff>

<commit_message>
working on notebooks preparation with logics
</commit_message>
<xml_diff>
--- a/notebooks/Questions_2024-05-31.xlsx
+++ b/notebooks/Questions_2024-05-31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABMI_Official\RCDST_Jupyter_webapp_Official\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9233ABFC-EE55-4168-98AB-C1B31FA69030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6230A6-354B-4EA1-A74D-623670F13BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="825" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11166,9 +11166,9 @@
   </sheetPr>
   <dimension ref="A1:AF63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>

</xml_diff>